<commit_message>
corrected encode-decode measurements in gbps
</commit_message>
<xml_diff>
--- a/measurements/measurements.xlsx
+++ b/measurements/measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14540" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14460" tabRatio="500" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="encode k=10,m=3, w=8" sheetId="2" r:id="rId1"/>
@@ -118,10 +118,10 @@
     <t>k=10 m=3 w=8 file=16MB</t>
   </si>
   <si>
-    <t>In MBps</t>
+    <t>decode(from K-M blocks)</t>
   </si>
   <si>
-    <t>decode(from K-M blocks)</t>
+    <t>In GBps</t>
   </si>
 </sst>
 </file>
@@ -294,7 +294,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -732,11 +731,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2109151544"/>
-        <c:axId val="2109158392"/>
+        <c:axId val="-2112224056"/>
+        <c:axId val="-2112137864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2109151544"/>
+        <c:axId val="-2112224056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,13 +757,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109158392"/>
+        <c:crossAx val="-2112137864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -772,7 +770,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109158392"/>
+        <c:axId val="-2112137864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -796,21 +794,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109151544"/>
+        <c:crossAx val="-2112224056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1071,11 +1067,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2137782232"/>
-        <c:axId val="2137783640"/>
+        <c:axId val="2138978104"/>
+        <c:axId val="2138611656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2137782232"/>
+        <c:axId val="2138978104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1084,7 +1080,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137783640"/>
+        <c:crossAx val="2138611656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1092,7 +1088,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2137783640"/>
+        <c:axId val="2138611656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1122,7 +1118,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137782232"/>
+        <c:crossAx val="2138978104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1390,11 +1386,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2112903560"/>
-        <c:axId val="2123307944"/>
+        <c:axId val="2138708216"/>
+        <c:axId val="2138337928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2112903560"/>
+        <c:axId val="2138708216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1403,7 +1399,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123307944"/>
+        <c:crossAx val="2138337928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1411,7 +1407,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123307944"/>
+        <c:axId val="2138337928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1430,7 +1426,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>MBps</a:t>
+                  <a:t>GBps</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1442,7 +1438,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112903560"/>
+        <c:crossAx val="2138708216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1489,7 +1485,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1927,11 +1922,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2107729800"/>
-        <c:axId val="2107724296"/>
+        <c:axId val="-2112175784"/>
+        <c:axId val="2138214936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2107729800"/>
+        <c:axId val="-2112175784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1953,13 +1948,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107724296"/>
+        <c:crossAx val="2138214936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1967,7 +1961,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2107724296"/>
+        <c:axId val="2138214936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1991,21 +1985,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107729800"/>
+        <c:crossAx val="-2112175784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2050,7 +2042,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2488,11 +2479,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2107669880"/>
-        <c:axId val="2107664376"/>
+        <c:axId val="-2112151784"/>
+        <c:axId val="2138319560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2107669880"/>
+        <c:axId val="-2112151784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2514,13 +2505,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107664376"/>
+        <c:crossAx val="2138319560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2528,7 +2518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2107664376"/>
+        <c:axId val="2138319560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2552,21 +2542,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107669880"/>
+        <c:crossAx val="-2112151784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3049,11 +3037,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2110171720"/>
-        <c:axId val="2110177208"/>
+        <c:axId val="2110268904"/>
+        <c:axId val="2110262984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110171720"/>
+        <c:axId val="2110268904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3081,7 +3069,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110177208"/>
+        <c:crossAx val="2110262984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3089,7 +3077,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110177208"/>
+        <c:axId val="2110262984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3120,7 +3108,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110171720"/>
+        <c:crossAx val="2110268904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3608,11 +3596,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2110219368"/>
-        <c:axId val="2110224856"/>
+        <c:axId val="2138346792"/>
+        <c:axId val="2138986008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110219368"/>
+        <c:axId val="2138346792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3640,7 +3628,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110224856"/>
+        <c:crossAx val="2138986008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3648,7 +3636,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110224856"/>
+        <c:axId val="2138986008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3679,7 +3667,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110219368"/>
+        <c:crossAx val="2138346792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4164,11 +4152,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2110266088"/>
-        <c:axId val="2110271576"/>
+        <c:axId val="-2111039176"/>
+        <c:axId val="2081072904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110266088"/>
+        <c:axId val="-2111039176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4196,7 +4184,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110271576"/>
+        <c:crossAx val="2081072904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4204,7 +4192,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110271576"/>
+        <c:axId val="2081072904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -4235,7 +4223,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110266088"/>
+        <c:crossAx val="-2111039176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4720,11 +4708,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2117654792"/>
-        <c:axId val="2117739640"/>
+        <c:axId val="2129663816"/>
+        <c:axId val="-2111401272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2117654792"/>
+        <c:axId val="2129663816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4752,7 +4740,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117739640"/>
+        <c:crossAx val="-2111401272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4760,7 +4748,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117739640"/>
+        <c:axId val="-2111401272"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4792,7 +4780,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117654792"/>
+        <c:crossAx val="2129663816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5280,11 +5268,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2122698840"/>
-        <c:axId val="2127474136"/>
+        <c:axId val="-2111074952"/>
+        <c:axId val="-2111069464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2122698840"/>
+        <c:axId val="-2111074952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5312,7 +5300,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127474136"/>
+        <c:crossAx val="-2111069464"/>
         <c:crossesAt val="0.1"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5320,7 +5308,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127474136"/>
+        <c:axId val="-2111069464"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5352,7 +5340,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122698840"/>
+        <c:crossAx val="-2111074952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5837,11 +5825,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2122477016"/>
-        <c:axId val="2126861864"/>
+        <c:axId val="2130004408"/>
+        <c:axId val="2122048952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2122477016"/>
+        <c:axId val="2130004408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5869,7 +5857,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126861864"/>
+        <c:crossAx val="2122048952"/>
         <c:crossesAt val="0.01"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5877,7 +5865,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126861864"/>
+        <c:axId val="2122048952"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5909,7 +5897,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122477016"/>
+        <c:crossAx val="2130004408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19125,7 +19113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
@@ -19147,8 +19135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N120" sqref="N120"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="M121" sqref="M121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -19164,7 +19152,7 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -20095,11 +20083,11 @@
         <v>21</v>
       </c>
       <c r="B114" s="1">
-        <f>B108-B107</f>
+        <f t="shared" ref="B114:C116" si="0">B108-B107</f>
         <v>2.4499999999999993</v>
       </c>
       <c r="C114" s="1">
-        <f>C108-C107</f>
+        <f t="shared" si="0"/>
         <v>1.5925000000000011</v>
       </c>
       <c r="D114" t="s">
@@ -20111,11 +20099,11 @@
         <v>22</v>
       </c>
       <c r="B115" s="1">
-        <f>B109-B108</f>
+        <f t="shared" si="0"/>
         <v>4.2025000000000006</v>
       </c>
       <c r="C115" s="1">
-        <f>C109-C108</f>
+        <f t="shared" si="0"/>
         <v>1.7850000000000001</v>
       </c>
       <c r="D115" t="s">
@@ -20127,11 +20115,11 @@
         <v>23</v>
       </c>
       <c r="B116" s="2">
-        <f>B110-B109</f>
+        <f t="shared" si="0"/>
         <v>16.062500000000004</v>
       </c>
       <c r="C116" s="2">
-        <f>C110-C109</f>
+        <f t="shared" si="0"/>
         <v>17.144999999999996</v>
       </c>
       <c r="D116" t="s">
@@ -20140,7 +20128,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -20148,11 +20136,11 @@
         <v>20</v>
       </c>
       <c r="B119" s="3">
-        <f>B112/16</f>
+        <f>B112*0.0625</f>
         <v>0.21531250000000002</v>
       </c>
       <c r="C119" s="3">
-        <f>C112/16</f>
+        <f>C112*0.0625</f>
         <v>8.6718750000000067E-2</v>
       </c>
       <c r="D119" t="s">
@@ -20164,11 +20152,11 @@
         <v>16</v>
       </c>
       <c r="B120" s="3">
-        <f t="shared" ref="B120:C123" si="0">B113/16</f>
+        <f t="shared" ref="B120:C123" si="1">B113*0.0625</f>
         <v>1.2959375</v>
       </c>
       <c r="C120" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.99484375000000003</v>
       </c>
       <c r="D120" t="s">
@@ -20180,11 +20168,11 @@
         <v>21</v>
       </c>
       <c r="B121" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.15312499999999996</v>
       </c>
       <c r="C121" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.9531250000000071E-2</v>
       </c>
       <c r="D121" t="s">
@@ -20196,11 +20184,11 @@
         <v>22</v>
       </c>
       <c r="B122" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.26265625000000004</v>
       </c>
       <c r="C122" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.11156250000000001</v>
       </c>
       <c r="D122" t="s">
@@ -20212,11 +20200,11 @@
         <v>23</v>
       </c>
       <c r="B123" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0039062500000002</v>
       </c>
       <c r="C123" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0715624999999998</v>
       </c>
       <c r="D123" t="s">

</xml_diff>

<commit_message>
updated measurements for 512KB
</commit_message>
<xml_diff>
--- a/measurements/measurements.xlsx
+++ b/measurements/measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="encode k=10,m=3, w=8" sheetId="2" r:id="rId1"/>
@@ -203,8 +203,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -239,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -253,6 +257,8 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -266,6 +272,8 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -303,6 +311,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -368,7 +377,7 @@
                     <c:v>0.0700000000000001</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.25</c:v>
+                    <c:v>0.0699999999999998</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>0.225</c:v>
@@ -452,7 +461,7 @@
                   <c:v>1.23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.14</c:v>
+                  <c:v>1.44</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2.135</c:v>
@@ -551,7 +560,7 @@
                   <c:v>0.0900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.155</c:v>
+                  <c:v>0.0800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.25</c:v>
@@ -616,7 +625,7 @@
                     <c:v>1.79</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>2.8975</c:v>
+                    <c:v>3.2075</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>3.7475</c:v>
@@ -709,7 +718,7 @@
                   <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4775</c:v>
+                  <c:v>0.1425</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.3075</c:v>
@@ -740,11 +749,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2112006440"/>
-        <c:axId val="-2112200024"/>
+        <c:axId val="2135397336"/>
+        <c:axId val="2122485864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2112006440"/>
+        <c:axId val="2135397336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -766,12 +775,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112200024"/>
+        <c:crossAx val="2122485864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -779,8 +789,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112200024"/>
+        <c:axId val="2122485864"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
         </c:scaling>
@@ -803,19 +814,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112006440"/>
+        <c:crossAx val="2135397336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -860,7 +873,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1076,11 +1088,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2109161128"/>
-        <c:axId val="2109141912"/>
+        <c:axId val="2121775816"/>
+        <c:axId val="2129144360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2109161128"/>
+        <c:axId val="2121775816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1089,7 +1101,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109141912"/>
+        <c:crossAx val="2129144360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1097,7 +1109,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109141912"/>
+        <c:axId val="2129144360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,14 +1132,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109161128"/>
+        <c:crossAx val="2121775816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1179,7 +1190,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1395,11 +1405,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2137179240"/>
-        <c:axId val="-2111325224"/>
+        <c:axId val="2129613320"/>
+        <c:axId val="2129078280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2137179240"/>
+        <c:axId val="2129613320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1408,7 +1418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111325224"/>
+        <c:crossAx val="2129078280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1416,7 +1426,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111325224"/>
+        <c:axId val="2129078280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1440,14 +1450,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137179240"/>
+        <c:crossAx val="2129613320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1494,6 +1503,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1559,7 +1569,7 @@
                     <c:v>0.1</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.27</c:v>
+                    <c:v>0.0599999999999999</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>0.2175</c:v>
@@ -1643,7 +1653,7 @@
                   <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.75</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.7675</c:v>
@@ -1742,7 +1752,7 @@
                   <c:v>0.0599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.185</c:v>
+                  <c:v>0.0900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.1925</c:v>
@@ -1807,7 +1817,7 @@
                     <c:v>1.7</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.8175</c:v>
+                    <c:v>2.0375</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>1.3675</c:v>
@@ -1900,7 +1910,7 @@
                   <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3275</c:v>
+                  <c:v>0.1925</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.4525</c:v>
@@ -1931,11 +1941,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2137046264"/>
-        <c:axId val="-2112416536"/>
+        <c:axId val="2135239640"/>
+        <c:axId val="2124021976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2137046264"/>
+        <c:axId val="2135239640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1957,21 +1967,23 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112416536"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="2124021976"/>
+        <c:crossesAt val="0.1"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112416536"/>
+        <c:axId val="2124021976"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
         </c:scaling>
@@ -1994,19 +2006,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137046264"/>
+        <c:crossAx val="2135239640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2051,6 +2065,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2116,7 +2131,7 @@
                     <c:v>0.05</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.275</c:v>
+                    <c:v>0.0299999999999999</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>0.37</c:v>
@@ -2200,7 +2215,7 @@
                   <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.505</c:v>
+                  <c:v>0.58</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.52</c:v>
@@ -2299,7 +2314,7 @@
                   <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13</c:v>
+                  <c:v>0.045</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.27</c:v>
@@ -2364,7 +2379,7 @@
                     <c:v>0.14</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>2.3775</c:v>
+                    <c:v>1.475</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>3.54</c:v>
@@ -2457,7 +2472,7 @@
                   <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3775</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.21</c:v>
@@ -2488,11 +2503,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2112299928"/>
-        <c:axId val="-2112584952"/>
+        <c:axId val="2122553720"/>
+        <c:axId val="2122343832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2112299928"/>
+        <c:axId val="2122553720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2514,21 +2529,23 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112584952"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="2122343832"/>
+        <c:crossesAt val="0.01"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112584952"/>
+        <c:axId val="2122343832"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
         </c:scaling>
@@ -2551,19 +2568,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112299928"/>
+        <c:crossAx val="2122553720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2608,6 +2627,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2673,7 +2693,7 @@
                     <c:v>0.0700000000000001</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.25</c:v>
+                    <c:v>0.0699999999999998</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>0.225</c:v>
@@ -2757,7 +2777,7 @@
                   <c:v>1.23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.14</c:v>
+                  <c:v>1.44</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2.135</c:v>
@@ -2856,7 +2876,7 @@
                   <c:v>0.0900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.155</c:v>
+                  <c:v>0.0800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.25</c:v>
@@ -2921,7 +2941,7 @@
                     <c:v>1.79</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>2.8975</c:v>
+                    <c:v>3.2075</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>3.7475</c:v>
@@ -3014,7 +3034,7 @@
                   <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4775</c:v>
+                  <c:v>0.1425</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.3075</c:v>
@@ -3045,11 +3065,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2105642536"/>
-        <c:axId val="-2110806440"/>
+        <c:axId val="2123452728"/>
+        <c:axId val="2122887544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105642536"/>
+        <c:axId val="2123452728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3071,12 +3091,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110806440"/>
+        <c:crossAx val="2122887544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3084,7 +3105,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2110806440"/>
+        <c:axId val="2122887544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3108,13 +3129,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105642536"/>
+        <c:crossAx val="2123452728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3161,6 +3183,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3229,7 +3252,7 @@
                     <c:v>0.1</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.27</c:v>
+                    <c:v>0.0599999999999999</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>0.2175</c:v>
@@ -3313,7 +3336,7 @@
                   <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.75</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.7675</c:v>
@@ -3412,7 +3435,7 @@
                   <c:v>0.0599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.185</c:v>
+                  <c:v>0.0900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.1925</c:v>
@@ -3477,7 +3500,7 @@
                     <c:v>1.7</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.8175</c:v>
+                    <c:v>2.0375</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>1.3675</c:v>
@@ -3570,7 +3593,7 @@
                   <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3275</c:v>
+                  <c:v>0.1925</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.4525</c:v>
@@ -3601,11 +3624,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2109138568"/>
-        <c:axId val="-2110944088"/>
+        <c:axId val="2110202024"/>
+        <c:axId val="-2112062376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2109138568"/>
+        <c:axId val="2110202024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3627,12 +3650,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110944088"/>
+        <c:crossAx val="-2112062376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3640,7 +3664,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2110944088"/>
+        <c:axId val="-2112062376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3664,13 +3688,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109138568"/>
+        <c:crossAx val="2110202024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3717,6 +3742,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3782,7 +3808,7 @@
                     <c:v>0.05</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.275</c:v>
+                    <c:v>0.0299999999999999</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>0.37</c:v>
@@ -3866,7 +3892,7 @@
                   <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.505</c:v>
+                  <c:v>0.58</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.52</c:v>
@@ -3965,7 +3991,7 @@
                   <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13</c:v>
+                  <c:v>0.045</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.27</c:v>
@@ -4030,7 +4056,7 @@
                     <c:v>0.14</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>2.3775</c:v>
+                    <c:v>1.475</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>3.54</c:v>
@@ -4123,7 +4149,7 @@
                   <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3775</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.21</c:v>
@@ -4154,11 +4180,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2110903640"/>
-        <c:axId val="-2110898152"/>
+        <c:axId val="2138321720"/>
+        <c:axId val="-2111940216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2110903640"/>
+        <c:axId val="2138321720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4180,12 +4206,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110898152"/>
+        <c:crossAx val="-2111940216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4193,7 +4220,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2110898152"/>
+        <c:axId val="-2111940216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -4217,13 +4244,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110903640"/>
+        <c:crossAx val="2138321720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4270,6 +4298,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4335,7 +4364,7 @@
                     <c:v>0.0700000000000001</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.25</c:v>
+                    <c:v>0.0699999999999998</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>0.225</c:v>
@@ -4419,7 +4448,7 @@
                   <c:v>1.23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.14</c:v>
+                  <c:v>1.44</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2.135</c:v>
@@ -4518,7 +4547,7 @@
                   <c:v>0.0900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.155</c:v>
+                  <c:v>0.0800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.25</c:v>
@@ -4583,7 +4612,7 @@
                     <c:v>1.79</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>2.8975</c:v>
+                    <c:v>3.2075</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>3.7475</c:v>
@@ -4676,7 +4705,7 @@
                   <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4775</c:v>
+                  <c:v>0.1425</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.3075</c:v>
@@ -4707,11 +4736,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2110857112"/>
-        <c:axId val="-2110851624"/>
+        <c:axId val="-2111926504"/>
+        <c:axId val="2122421960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2110857112"/>
+        <c:axId val="-2111926504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4733,12 +4762,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110851624"/>
+        <c:crossAx val="2122421960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4746,7 +4776,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2110851624"/>
+        <c:axId val="2122421960"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4771,13 +4801,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110857112"/>
+        <c:crossAx val="-2111926504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4824,6 +4855,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4892,7 +4924,7 @@
                     <c:v>0.1</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.27</c:v>
+                    <c:v>0.0599999999999999</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>0.2175</c:v>
@@ -4976,7 +5008,7 @@
                   <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.75</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.7675</c:v>
@@ -5075,7 +5107,7 @@
                   <c:v>0.0599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.185</c:v>
+                  <c:v>0.0900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.1925</c:v>
@@ -5140,7 +5172,7 @@
                     <c:v>1.7</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.8175</c:v>
+                    <c:v>2.0375</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>1.3675</c:v>
@@ -5233,7 +5265,7 @@
                   <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3275</c:v>
+                  <c:v>0.1925</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.4525</c:v>
@@ -5264,11 +5296,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2138262952"/>
-        <c:axId val="2138634120"/>
+        <c:axId val="2124034536"/>
+        <c:axId val="2124035352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2138262952"/>
+        <c:axId val="2124034536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5290,12 +5322,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138634120"/>
+        <c:crossAx val="2124035352"/>
         <c:crossesAt val="0.1"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5303,7 +5336,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2138634120"/>
+        <c:axId val="2124035352"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5328,13 +5361,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138262952"/>
+        <c:crossAx val="2124034536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5381,6 +5415,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5446,7 +5481,7 @@
                     <c:v>0.05</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.275</c:v>
+                    <c:v>0.0299999999999999</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>0.37</c:v>
@@ -5530,7 +5565,7 @@
                   <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.505</c:v>
+                  <c:v>0.58</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.52</c:v>
@@ -5629,7 +5664,7 @@
                   <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13</c:v>
+                  <c:v>0.045</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.27</c:v>
@@ -5694,7 +5729,7 @@
                     <c:v>0.14</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>2.3775</c:v>
+                    <c:v>1.475</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>3.54</c:v>
@@ -5787,7 +5822,7 @@
                   <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3775</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.21</c:v>
@@ -5818,11 +5853,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2112270376"/>
-        <c:axId val="2110242872"/>
+        <c:axId val="2136128728"/>
+        <c:axId val="2136105112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2112270376"/>
+        <c:axId val="2136128728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5844,12 +5879,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110242872"/>
+        <c:crossAx val="2136105112"/>
         <c:crossesAt val="0.01"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5857,7 +5893,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110242872"/>
+        <c:axId val="2136105112"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5882,13 +5918,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112270376"/>
+        <c:crossAx val="2136128728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5947,13 +5984,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
       <xdr:row>116</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>143</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6600,8 +6637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M116"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103:A116"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M136" sqref="M136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6665,7 +6702,7 @@
         <v>1.33</v>
       </c>
       <c r="G2">
-        <v>2.87</v>
+        <v>1.51</v>
       </c>
       <c r="H2">
         <v>2.2000000000000002</v>
@@ -6700,7 +6737,7 @@
         <v>1.17</v>
       </c>
       <c r="G3">
-        <v>2.21</v>
+        <v>1.51</v>
       </c>
       <c r="H3">
         <v>2.87</v>
@@ -6735,7 +6772,7 @@
         <v>1.34</v>
       </c>
       <c r="G4">
-        <v>2.11</v>
+        <v>1.4</v>
       </c>
       <c r="H4">
         <v>2.4300000000000002</v>
@@ -6770,7 +6807,7 @@
         <v>1.55</v>
       </c>
       <c r="G5">
-        <v>4.6900000000000004</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <v>2.81</v>
@@ -6805,7 +6842,7 @@
         <v>1.98</v>
       </c>
       <c r="G6">
-        <v>2.75</v>
+        <v>1.4</v>
       </c>
       <c r="H6">
         <v>2.1</v>
@@ -6840,7 +6877,7 @@
         <v>1.18</v>
       </c>
       <c r="G7">
-        <v>1.9</v>
+        <v>1.42</v>
       </c>
       <c r="H7">
         <v>2.64</v>
@@ -6875,7 +6912,7 @@
         <v>1.31</v>
       </c>
       <c r="G8">
-        <v>2.73</v>
+        <v>3.28</v>
       </c>
       <c r="H8">
         <v>2.9</v>
@@ -6910,7 +6947,7 @@
         <v>1.3</v>
       </c>
       <c r="G9">
-        <v>1.95</v>
+        <v>1.48</v>
       </c>
       <c r="H9">
         <v>2.14</v>
@@ -6945,7 +6982,7 @@
         <v>1.23</v>
       </c>
       <c r="G10">
-        <v>1.95</v>
+        <v>1.39</v>
       </c>
       <c r="H10">
         <v>2.46</v>
@@ -6980,7 +7017,7 @@
         <v>1.36</v>
       </c>
       <c r="G11">
-        <v>2.15</v>
+        <v>1.61</v>
       </c>
       <c r="H11">
         <v>4.0599999999999996</v>
@@ -7015,7 +7052,7 @@
         <v>1.27</v>
       </c>
       <c r="G12">
-        <v>2.15</v>
+        <v>1.66</v>
       </c>
       <c r="H12">
         <v>2.1800000000000002</v>
@@ -7050,7 +7087,7 @@
         <v>1.66</v>
       </c>
       <c r="G13">
-        <v>2.0299999999999998</v>
+        <v>2.15</v>
       </c>
       <c r="H13">
         <v>2.58</v>
@@ -7085,7 +7122,7 @@
         <v>1.38</v>
       </c>
       <c r="G14">
-        <v>1.92</v>
+        <v>1.58</v>
       </c>
       <c r="H14">
         <v>2.89</v>
@@ -7120,7 +7157,7 @@
         <v>1.19</v>
       </c>
       <c r="G15">
-        <v>3.2</v>
+        <v>1.61</v>
       </c>
       <c r="H15">
         <v>3.06</v>
@@ -7155,7 +7192,7 @@
         <v>1.84</v>
       </c>
       <c r="G16">
-        <v>2.19</v>
+        <v>1.39</v>
       </c>
       <c r="H16">
         <v>4.32</v>
@@ -7190,7 +7227,7 @@
         <v>1.26</v>
       </c>
       <c r="G17">
-        <v>3.24</v>
+        <v>1.67</v>
       </c>
       <c r="H17">
         <v>2.14</v>
@@ -7225,7 +7262,7 @@
         <v>1.19</v>
       </c>
       <c r="G18">
-        <v>1.99</v>
+        <v>1.4</v>
       </c>
       <c r="H18">
         <v>2.39</v>
@@ -7260,7 +7297,7 @@
         <v>1.18</v>
       </c>
       <c r="G19">
-        <v>2.17</v>
+        <v>1.39</v>
       </c>
       <c r="H19">
         <v>2.7</v>
@@ -7295,7 +7332,7 @@
         <v>1.32</v>
       </c>
       <c r="G20">
-        <v>2.04</v>
+        <v>1.61</v>
       </c>
       <c r="H20">
         <v>2.34</v>
@@ -7330,7 +7367,7 @@
         <v>1.23</v>
       </c>
       <c r="G21">
-        <v>2.2999999999999998</v>
+        <v>1.44</v>
       </c>
       <c r="H21">
         <v>2.04</v>
@@ -7365,7 +7402,7 @@
         <v>1.18</v>
       </c>
       <c r="G22">
-        <v>2.0699999999999998</v>
+        <v>1.46</v>
       </c>
       <c r="H22">
         <v>2.4700000000000002</v>
@@ -7400,7 +7437,7 @@
         <v>1.23</v>
       </c>
       <c r="G23">
-        <v>4.28</v>
+        <v>1.54</v>
       </c>
       <c r="H23">
         <v>2.33</v>
@@ -7435,7 +7472,7 @@
         <v>1.53</v>
       </c>
       <c r="G24">
-        <v>2.34</v>
+        <v>1.39</v>
       </c>
       <c r="H24">
         <v>3.11</v>
@@ -7470,7 +7507,7 @@
         <v>1.43</v>
       </c>
       <c r="G25">
-        <v>2.72</v>
+        <v>1.44</v>
       </c>
       <c r="H25">
         <v>2.2799999999999998</v>
@@ -7505,7 +7542,7 @@
         <v>1.23</v>
       </c>
       <c r="G26">
-        <v>2.82</v>
+        <v>1.37</v>
       </c>
       <c r="H26">
         <v>2.33</v>
@@ -7540,7 +7577,7 @@
         <v>1.18</v>
       </c>
       <c r="G27">
-        <v>2.11</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="H27">
         <v>2.91</v>
@@ -7575,7 +7612,7 @@
         <v>1.89</v>
       </c>
       <c r="G28">
-        <v>2.71</v>
+        <v>2.38</v>
       </c>
       <c r="H28">
         <v>2.0499999999999998</v>
@@ -7610,7 +7647,7 @@
         <v>1.28</v>
       </c>
       <c r="G29">
-        <v>2.25</v>
+        <v>1.5</v>
       </c>
       <c r="H29">
         <v>2.06</v>
@@ -7645,7 +7682,7 @@
         <v>1.17</v>
       </c>
       <c r="G30">
-        <v>2.38</v>
+        <v>1.5</v>
       </c>
       <c r="H30">
         <v>4.34</v>
@@ -7680,7 +7717,7 @@
         <v>1.17</v>
       </c>
       <c r="G31">
-        <v>2.76</v>
+        <v>1.51</v>
       </c>
       <c r="H31">
         <v>2.29</v>
@@ -7715,7 +7752,7 @@
         <v>1.26</v>
       </c>
       <c r="G32">
-        <v>2.5499999999999998</v>
+        <v>1.64</v>
       </c>
       <c r="H32">
         <v>2.34</v>
@@ -7750,7 +7787,7 @@
         <v>1.37</v>
       </c>
       <c r="G33">
-        <v>2.14</v>
+        <v>1.44</v>
       </c>
       <c r="H33">
         <v>2.48</v>
@@ -7785,7 +7822,7 @@
         <v>1.18</v>
       </c>
       <c r="G34">
-        <v>2.17</v>
+        <v>1.49</v>
       </c>
       <c r="H34">
         <v>2.34</v>
@@ -7820,7 +7857,7 @@
         <v>1.25</v>
       </c>
       <c r="G35">
-        <v>2.2400000000000002</v>
+        <v>1.5</v>
       </c>
       <c r="H35">
         <v>2.0699999999999998</v>
@@ -7855,7 +7892,7 @@
         <v>1.24</v>
       </c>
       <c r="G36">
-        <v>2.2200000000000002</v>
+        <v>1.66</v>
       </c>
       <c r="H36">
         <v>2.12</v>
@@ -7890,7 +7927,7 @@
         <v>1.26</v>
       </c>
       <c r="G37">
-        <v>2.0499999999999998</v>
+        <v>1.75</v>
       </c>
       <c r="H37">
         <v>2.88</v>
@@ -7925,7 +7962,7 @@
         <v>1.23</v>
       </c>
       <c r="G38">
-        <v>2.2000000000000002</v>
+        <v>1.38</v>
       </c>
       <c r="H38">
         <v>2.69</v>
@@ -7960,7 +7997,7 @@
         <v>1.17</v>
       </c>
       <c r="G39">
-        <v>3.07</v>
+        <v>1.63</v>
       </c>
       <c r="H39">
         <v>2.25</v>
@@ -7995,7 +8032,7 @@
         <v>1.19</v>
       </c>
       <c r="G40">
-        <v>2.12</v>
+        <v>1.37</v>
       </c>
       <c r="H40">
         <v>2.15</v>
@@ -8030,7 +8067,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="G41">
-        <v>2.77</v>
+        <v>1.39</v>
       </c>
       <c r="H41">
         <v>2.04</v>
@@ -8065,7 +8102,7 @@
         <v>1.2</v>
       </c>
       <c r="G42">
-        <v>2.94</v>
+        <v>1.39</v>
       </c>
       <c r="H42">
         <v>4.74</v>
@@ -8100,7 +8137,7 @@
         <v>1.19</v>
       </c>
       <c r="G43">
-        <v>2.33</v>
+        <v>1.7</v>
       </c>
       <c r="H43">
         <v>2.2799999999999998</v>
@@ -8135,7 +8172,7 @@
         <v>1.24</v>
       </c>
       <c r="G44">
-        <v>2.09</v>
+        <v>1.47</v>
       </c>
       <c r="H44">
         <v>2.17</v>
@@ -8170,7 +8207,7 @@
         <v>1.19</v>
       </c>
       <c r="G45">
-        <v>2.2599999999999998</v>
+        <v>2.04</v>
       </c>
       <c r="H45">
         <v>2.04</v>
@@ -8205,7 +8242,7 @@
         <v>1.33</v>
       </c>
       <c r="G46">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="H46">
         <v>1.95</v>
@@ -8240,7 +8277,7 @@
         <v>1.2</v>
       </c>
       <c r="G47">
-        <v>2.09</v>
+        <v>1.43</v>
       </c>
       <c r="H47">
         <v>2.06</v>
@@ -8275,7 +8312,7 @@
         <v>1.22</v>
       </c>
       <c r="G48">
-        <v>2.0699999999999998</v>
+        <v>1.77</v>
       </c>
       <c r="H48">
         <v>1.99</v>
@@ -8310,7 +8347,7 @@
         <v>1.29</v>
       </c>
       <c r="G49">
-        <v>2.0299999999999998</v>
+        <v>1.54</v>
       </c>
       <c r="H49">
         <v>2.35</v>
@@ -8345,7 +8382,7 @@
         <v>1.57</v>
       </c>
       <c r="G50">
-        <v>2.16</v>
+        <v>4.87</v>
       </c>
       <c r="H50">
         <v>2.4</v>
@@ -8380,7 +8417,7 @@
         <v>1.77</v>
       </c>
       <c r="G51">
-        <v>2.38</v>
+        <v>1.5</v>
       </c>
       <c r="H51">
         <v>2.59</v>
@@ -8415,7 +8452,7 @@
         <v>1.28</v>
       </c>
       <c r="G52">
-        <v>1.89</v>
+        <v>1.41</v>
       </c>
       <c r="H52">
         <v>2.34</v>
@@ -8450,7 +8487,7 @@
         <v>1.32</v>
       </c>
       <c r="G53">
-        <v>2.35</v>
+        <v>1.48</v>
       </c>
       <c r="H53">
         <v>4.28</v>
@@ -8485,7 +8522,7 @@
         <v>1.56</v>
       </c>
       <c r="G54">
-        <v>3.31</v>
+        <v>1.74</v>
       </c>
       <c r="H54">
         <v>2.25</v>
@@ -8520,7 +8557,7 @@
         <v>1.77</v>
       </c>
       <c r="G55">
-        <v>2.14</v>
+        <v>1.4</v>
       </c>
       <c r="H55">
         <v>2.41</v>
@@ -8555,7 +8592,7 @@
         <v>1.3</v>
       </c>
       <c r="G56">
-        <v>2.61</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="H56">
         <v>1.97</v>
@@ -8590,7 +8627,7 @@
         <v>1.25</v>
       </c>
       <c r="G57">
-        <v>2.78</v>
+        <v>1.59</v>
       </c>
       <c r="H57">
         <v>2.54</v>
@@ -8625,7 +8662,7 @@
         <v>1.57</v>
       </c>
       <c r="G58">
-        <v>2.78</v>
+        <v>1.72</v>
       </c>
       <c r="H58">
         <v>1.91</v>
@@ -8660,7 +8697,7 @@
         <v>1.18</v>
       </c>
       <c r="G59">
-        <v>2.29</v>
+        <v>1.52</v>
       </c>
       <c r="H59">
         <v>2.93</v>
@@ -8695,7 +8732,7 @@
         <v>1.86</v>
       </c>
       <c r="G60">
-        <v>2.44</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="H60">
         <v>3.11</v>
@@ -8730,7 +8767,7 @@
         <v>1.28</v>
       </c>
       <c r="G61">
-        <v>2.4300000000000002</v>
+        <v>1.49</v>
       </c>
       <c r="H61">
         <v>2.64</v>
@@ -8765,7 +8802,7 @@
         <v>1.45</v>
       </c>
       <c r="G62">
-        <v>3.2</v>
+        <v>1.68</v>
       </c>
       <c r="H62">
         <v>2.96</v>
@@ -8800,7 +8837,7 @@
         <v>1.66</v>
       </c>
       <c r="G63">
-        <v>2.16</v>
+        <v>1.8</v>
       </c>
       <c r="H63">
         <v>2.46</v>
@@ -8870,7 +8907,7 @@
         <v>1.68</v>
       </c>
       <c r="G65">
-        <v>4</v>
+        <v>1.89</v>
       </c>
       <c r="H65">
         <v>2.12</v>
@@ -8905,7 +8942,7 @@
         <v>1.28</v>
       </c>
       <c r="G66">
-        <v>2.5499999999999998</v>
+        <v>1.52</v>
       </c>
       <c r="H66">
         <v>4.6500000000000004</v>
@@ -8940,7 +8977,7 @@
         <v>1.35</v>
       </c>
       <c r="G67">
-        <v>2.2599999999999998</v>
+        <v>1.43</v>
       </c>
       <c r="H67">
         <v>2.4</v>
@@ -8975,7 +9012,7 @@
         <v>1.52</v>
       </c>
       <c r="G68">
-        <v>2.16</v>
+        <v>1.59</v>
       </c>
       <c r="H68">
         <v>1.92</v>
@@ -9010,7 +9047,7 @@
         <v>1.29</v>
       </c>
       <c r="G69">
-        <v>5.67</v>
+        <v>1.4</v>
       </c>
       <c r="H69">
         <v>2.5299999999999998</v>
@@ -9045,7 +9082,7 @@
         <v>1.27</v>
       </c>
       <c r="G70">
-        <v>2.74</v>
+        <v>1.85</v>
       </c>
       <c r="H70">
         <v>1.97</v>
@@ -9080,7 +9117,7 @@
         <v>3.32</v>
       </c>
       <c r="G71">
-        <v>2.5299999999999998</v>
+        <v>1.58</v>
       </c>
       <c r="H71">
         <v>2.64</v>
@@ -9115,7 +9152,7 @@
         <v>1.43</v>
       </c>
       <c r="G72">
-        <v>2.31</v>
+        <v>1.65</v>
       </c>
       <c r="H72">
         <v>2.65</v>
@@ -9150,7 +9187,7 @@
         <v>1.89</v>
       </c>
       <c r="G73">
-        <v>2.0099999999999998</v>
+        <v>1.73</v>
       </c>
       <c r="H73">
         <v>3.08</v>
@@ -9185,7 +9222,7 @@
         <v>1.45</v>
       </c>
       <c r="G74">
-        <v>2.25</v>
+        <v>1.59</v>
       </c>
       <c r="H74">
         <v>2.34</v>
@@ -9220,7 +9257,7 @@
         <v>1.31</v>
       </c>
       <c r="G75">
-        <v>2.08</v>
+        <v>1.54</v>
       </c>
       <c r="H75">
         <v>2.48</v>
@@ -9255,7 +9292,7 @@
         <v>1.37</v>
       </c>
       <c r="G76">
-        <v>3.23</v>
+        <v>1.63</v>
       </c>
       <c r="H76">
         <v>2.52</v>
@@ -9290,7 +9327,7 @@
         <v>1.36</v>
       </c>
       <c r="G77">
-        <v>2.31</v>
+        <v>1.46</v>
       </c>
       <c r="H77">
         <v>2.63</v>
@@ -9325,7 +9362,7 @@
         <v>1.97</v>
       </c>
       <c r="G78">
-        <v>2.4900000000000002</v>
+        <v>1.41</v>
       </c>
       <c r="H78">
         <v>2.11</v>
@@ -9360,7 +9397,7 @@
         <v>1.28</v>
       </c>
       <c r="G79">
-        <v>2.27</v>
+        <v>1.45</v>
       </c>
       <c r="H79">
         <v>2.81</v>
@@ -9395,7 +9432,7 @@
         <v>1.33</v>
       </c>
       <c r="G80">
-        <v>3.08</v>
+        <v>1.53</v>
       </c>
       <c r="H80">
         <v>2.12</v>
@@ -9430,7 +9467,7 @@
         <v>1.21</v>
       </c>
       <c r="G81">
-        <v>3.23</v>
+        <v>1.45</v>
       </c>
       <c r="H81">
         <v>2.0099999999999998</v>
@@ -9465,7 +9502,7 @@
         <v>1.62</v>
       </c>
       <c r="G82">
-        <v>5.44</v>
+        <v>1.47</v>
       </c>
       <c r="H82">
         <v>1.91</v>
@@ -9500,7 +9537,7 @@
         <v>1.37</v>
       </c>
       <c r="G83">
-        <v>2.41</v>
+        <v>1.61</v>
       </c>
       <c r="H83">
         <v>1.94</v>
@@ -9535,7 +9572,7 @@
         <v>2</v>
       </c>
       <c r="G84">
-        <v>2.87</v>
+        <v>1.49</v>
       </c>
       <c r="H84">
         <v>3.24</v>
@@ -9570,7 +9607,7 @@
         <v>1.33</v>
       </c>
       <c r="G85">
-        <v>1.92</v>
+        <v>1.73</v>
       </c>
       <c r="H85">
         <v>2.29</v>
@@ -9605,7 +9642,7 @@
         <v>1.24</v>
       </c>
       <c r="G86">
-        <v>2.94</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="H86">
         <v>1.94</v>
@@ -9640,7 +9677,7 @@
         <v>1.28</v>
       </c>
       <c r="G87">
-        <v>2.44</v>
+        <v>1.59</v>
       </c>
       <c r="H87">
         <v>2.33</v>
@@ -9675,7 +9712,7 @@
         <v>1.18</v>
       </c>
       <c r="G88">
-        <v>1.95</v>
+        <v>1.78</v>
       </c>
       <c r="H88">
         <v>1.91</v>
@@ -9710,7 +9747,7 @@
         <v>1.32</v>
       </c>
       <c r="G89">
-        <v>2.95</v>
+        <v>1.51</v>
       </c>
       <c r="H89">
         <v>2.44</v>
@@ -9745,7 +9782,7 @@
         <v>1.67</v>
       </c>
       <c r="G90">
-        <v>2.23</v>
+        <v>1.39</v>
       </c>
       <c r="H90">
         <v>2.39</v>
@@ -9780,7 +9817,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="G91">
-        <v>3.07</v>
+        <v>1.54</v>
       </c>
       <c r="H91">
         <v>2.1800000000000002</v>
@@ -9815,7 +9852,7 @@
         <v>1.35</v>
       </c>
       <c r="G92">
-        <v>1.93</v>
+        <v>1.48</v>
       </c>
       <c r="H92">
         <v>1.95</v>
@@ -9850,7 +9887,7 @@
         <v>1.48</v>
       </c>
       <c r="G93">
-        <v>2.84</v>
+        <v>1.43</v>
       </c>
       <c r="H93">
         <v>2.31</v>
@@ -9885,7 +9922,7 @@
         <v>1.53</v>
       </c>
       <c r="G94">
-        <v>1.99</v>
+        <v>1.4</v>
       </c>
       <c r="H94">
         <v>2.68</v>
@@ -9920,7 +9957,7 @@
         <v>1.39</v>
       </c>
       <c r="G95">
-        <v>2.98</v>
+        <v>1.42</v>
       </c>
       <c r="H95">
         <v>2.38</v>
@@ -9955,7 +9992,7 @@
         <v>1.34</v>
       </c>
       <c r="G96">
-        <v>2.48</v>
+        <v>1.53</v>
       </c>
       <c r="H96">
         <v>2.67</v>
@@ -9990,7 +10027,7 @@
         <v>1.72</v>
       </c>
       <c r="G97">
-        <v>2.19</v>
+        <v>1.52</v>
       </c>
       <c r="H97">
         <v>4.79</v>
@@ -10025,7 +10062,7 @@
         <v>1.38</v>
       </c>
       <c r="G98">
-        <v>2.2200000000000002</v>
+        <v>1.67</v>
       </c>
       <c r="H98">
         <v>2.92</v>
@@ -10060,7 +10097,7 @@
         <v>1.62</v>
       </c>
       <c r="G99">
-        <v>2.9</v>
+        <v>1.52</v>
       </c>
       <c r="H99">
         <v>2.94</v>
@@ -10095,7 +10132,7 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="G100">
-        <v>2.23</v>
+        <v>1.5</v>
       </c>
       <c r="H100">
         <v>6.44</v>
@@ -10130,7 +10167,7 @@
         <v>1.61</v>
       </c>
       <c r="G101">
-        <v>2.1800000000000002</v>
+        <v>1.48</v>
       </c>
       <c r="H101">
         <v>2.27</v>
@@ -10174,7 +10211,7 @@
       </c>
       <c r="G103">
         <f t="shared" si="0"/>
-        <v>2.5282999999999989</v>
+        <v>1.6352999999999998</v>
       </c>
       <c r="H103">
         <f t="shared" si="0"/>
@@ -10223,7 +10260,7 @@
       </c>
       <c r="G104">
         <f t="shared" si="1"/>
-        <v>0.66255558943451409</v>
+        <v>0.42238011268993303</v>
       </c>
       <c r="H104">
         <f t="shared" si="1"/>
@@ -10272,7 +10309,7 @@
       </c>
       <c r="G106">
         <f t="shared" si="2"/>
-        <v>1.89</v>
+        <v>1.37</v>
       </c>
       <c r="H106">
         <f t="shared" si="2"/>
@@ -10321,7 +10358,7 @@
       </c>
       <c r="G107">
         <f t="shared" si="3"/>
-        <v>2.14</v>
+        <v>1.44</v>
       </c>
       <c r="H107">
         <f t="shared" si="3"/>
@@ -10370,7 +10407,7 @@
       </c>
       <c r="G108">
         <f t="shared" si="4"/>
-        <v>2.2949999999999999</v>
+        <v>1.52</v>
       </c>
       <c r="H108">
         <f t="shared" si="4"/>
@@ -10419,7 +10456,7 @@
       </c>
       <c r="G109">
         <f t="shared" si="5"/>
-        <v>2.7725</v>
+        <v>1.6624999999999999</v>
       </c>
       <c r="H109">
         <f t="shared" si="5"/>
@@ -10468,7 +10505,7 @@
       </c>
       <c r="G110">
         <f t="shared" si="6"/>
-        <v>5.67</v>
+        <v>4.87</v>
       </c>
       <c r="H110">
         <f t="shared" si="6"/>
@@ -10517,7 +10554,7 @@
       </c>
       <c r="G112" s="3">
         <f t="shared" si="7"/>
-        <v>0.25000000000000022</v>
+        <v>6.999999999999984E-2</v>
       </c>
       <c r="H112" s="3">
         <f t="shared" si="7"/>
@@ -10569,7 +10606,7 @@
       </c>
       <c r="G113" s="1">
         <f t="shared" si="8"/>
-        <v>2.14</v>
+        <v>1.44</v>
       </c>
       <c r="H113" s="1">
         <f t="shared" si="8"/>
@@ -10621,7 +10658,7 @@
       </c>
       <c r="G114" s="1">
         <f t="shared" si="9"/>
-        <v>0.1549999999999998</v>
+        <v>8.0000000000000071E-2</v>
       </c>
       <c r="H114" s="1">
         <f t="shared" si="9"/>
@@ -10673,7 +10710,7 @@
       </c>
       <c r="G115" s="1">
         <f t="shared" si="10"/>
-        <v>0.47750000000000004</v>
+        <v>0.14249999999999985</v>
       </c>
       <c r="H115" s="1">
         <f t="shared" si="10"/>
@@ -10725,7 +10762,7 @@
       </c>
       <c r="G116" s="2">
         <f t="shared" si="11"/>
-        <v>2.8975</v>
+        <v>3.2075000000000005</v>
       </c>
       <c r="H116" s="2">
         <f t="shared" si="11"/>
@@ -10768,8 +10805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M116"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10833,7 +10870,7 @@
         <v>0.79</v>
       </c>
       <c r="G2">
-        <v>2.71</v>
+        <v>1.18</v>
       </c>
       <c r="H2">
         <v>1.78</v>
@@ -10868,7 +10905,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="G3">
-        <v>2.48</v>
+        <v>0.91</v>
       </c>
       <c r="H3">
         <v>2.77</v>
@@ -10903,7 +10940,7 @@
         <v>1.05</v>
       </c>
       <c r="G4">
-        <v>2.2799999999999998</v>
+        <v>1.05</v>
       </c>
       <c r="H4">
         <v>2.17</v>
@@ -10938,7 +10975,7 @@
         <v>0.76</v>
       </c>
       <c r="G5">
-        <v>1.76</v>
+        <v>1.62</v>
       </c>
       <c r="H5">
         <v>2.66</v>
@@ -10973,7 +11010,7 @@
         <v>0.89</v>
       </c>
       <c r="G6">
-        <v>2.71</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="H6">
         <v>2.19</v>
@@ -11008,7 +11045,7 @@
         <v>0.98</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>0.97</v>
       </c>
       <c r="H7">
         <v>1.82</v>
@@ -11043,7 +11080,7 @@
         <v>1.45</v>
       </c>
       <c r="G8">
-        <v>2.2599999999999998</v>
+        <v>1.03</v>
       </c>
       <c r="H8">
         <v>1.95</v>
@@ -11078,7 +11115,7 @@
         <v>0.73</v>
       </c>
       <c r="G9">
-        <v>1.85</v>
+        <v>1.22</v>
       </c>
       <c r="H9">
         <v>2.0299999999999998</v>
@@ -11113,7 +11150,7 @@
         <v>0.78</v>
       </c>
       <c r="G10">
-        <v>1.94</v>
+        <v>0.88</v>
       </c>
       <c r="H10">
         <v>2.2000000000000002</v>
@@ -11148,7 +11185,7 @@
         <v>0.96</v>
       </c>
       <c r="G11">
-        <v>1.91</v>
+        <v>1.7</v>
       </c>
       <c r="H11">
         <v>2.14</v>
@@ -11183,7 +11220,7 @@
         <v>1.07</v>
       </c>
       <c r="G12">
-        <v>2.37</v>
+        <v>1.27</v>
       </c>
       <c r="H12">
         <v>2.5099999999999998</v>
@@ -11218,7 +11255,7 @@
         <v>1.01</v>
       </c>
       <c r="G13">
-        <v>1.75</v>
+        <v>1.04</v>
       </c>
       <c r="H13">
         <v>1.84</v>
@@ -11253,7 +11290,7 @@
         <v>0.9</v>
       </c>
       <c r="G14">
-        <v>1.75</v>
+        <v>3</v>
       </c>
       <c r="H14">
         <v>2.12</v>
@@ -11288,7 +11325,7 @@
         <v>2.75</v>
       </c>
       <c r="G15">
-        <v>1.66</v>
+        <v>0.98</v>
       </c>
       <c r="H15">
         <v>2.4300000000000002</v>
@@ -11323,7 +11360,7 @@
         <v>0.93</v>
       </c>
       <c r="G16">
-        <v>1.99</v>
+        <v>1.44</v>
       </c>
       <c r="H16">
         <v>1.67</v>
@@ -11358,7 +11395,7 @@
         <v>0.91</v>
       </c>
       <c r="G17">
-        <v>1.65</v>
+        <v>0.95</v>
       </c>
       <c r="H17">
         <v>1.6</v>
@@ -11393,7 +11430,7 @@
         <v>0.79</v>
       </c>
       <c r="G18">
-        <v>1.96</v>
+        <v>0.95</v>
       </c>
       <c r="H18">
         <v>1.9</v>
@@ -11428,7 +11465,7 @@
         <v>0.75</v>
       </c>
       <c r="G19">
-        <v>1.88</v>
+        <v>0.94</v>
       </c>
       <c r="H19">
         <v>1.93</v>
@@ -11463,7 +11500,7 @@
         <v>0.79</v>
       </c>
       <c r="G20">
-        <v>2.0099999999999998</v>
+        <v>3.26</v>
       </c>
       <c r="H20">
         <v>2.46</v>
@@ -11498,7 +11535,7 @@
         <v>1.05</v>
       </c>
       <c r="G21">
-        <v>2.0499999999999998</v>
+        <v>0.95</v>
       </c>
       <c r="H21">
         <v>1.72</v>
@@ -11533,7 +11570,7 @@
         <v>0.74</v>
       </c>
       <c r="G22">
-        <v>1.48</v>
+        <v>0.98</v>
       </c>
       <c r="H22">
         <v>1.77</v>
@@ -11568,7 +11605,7 @@
         <v>0.72</v>
       </c>
       <c r="G23">
-        <v>2.02</v>
+        <v>1.55</v>
       </c>
       <c r="H23">
         <v>2.65</v>
@@ -11603,7 +11640,7 @@
         <v>0.84</v>
       </c>
       <c r="G24">
-        <v>1.65</v>
+        <v>0.92</v>
       </c>
       <c r="H24">
         <v>1.74</v>
@@ -11638,7 +11675,7 @@
         <v>0.78</v>
       </c>
       <c r="G25">
-        <v>2.11</v>
+        <v>0.9</v>
       </c>
       <c r="H25">
         <v>2.2000000000000002</v>
@@ -11673,7 +11710,7 @@
         <v>1.22</v>
       </c>
       <c r="G26">
-        <v>1.63</v>
+        <v>0.89</v>
       </c>
       <c r="H26">
         <v>2.66</v>
@@ -11708,7 +11745,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="G27">
-        <v>1.77</v>
+        <v>0.97</v>
       </c>
       <c r="H27">
         <v>1.8</v>
@@ -11743,7 +11780,7 @@
         <v>0.69</v>
       </c>
       <c r="G28">
-        <v>2.4300000000000002</v>
+        <v>0.9</v>
       </c>
       <c r="H28">
         <v>1.6</v>
@@ -11778,7 +11815,7 @@
         <v>0.69</v>
       </c>
       <c r="G29">
-        <v>1.61</v>
+        <v>1</v>
       </c>
       <c r="H29">
         <v>2.1800000000000002</v>
@@ -11813,7 +11850,7 @@
         <v>0.96</v>
       </c>
       <c r="G30">
-        <v>2.2599999999999998</v>
+        <v>0.88</v>
       </c>
       <c r="H30">
         <v>1.64</v>
@@ -11848,7 +11885,7 @@
         <v>1.22</v>
       </c>
       <c r="G31">
-        <v>1.86</v>
+        <v>0.98</v>
       </c>
       <c r="H31">
         <v>2.77</v>
@@ -11883,7 +11920,7 @@
         <v>1.18</v>
       </c>
       <c r="G32">
-        <v>2.16</v>
+        <v>0.92</v>
       </c>
       <c r="H32">
         <v>1.66</v>
@@ -11918,7 +11955,7 @@
         <v>0.73</v>
       </c>
       <c r="G33">
-        <v>2.15</v>
+        <v>0.96</v>
       </c>
       <c r="H33">
         <v>1.78</v>
@@ -11953,7 +11990,7 @@
         <v>0.77</v>
       </c>
       <c r="G34">
-        <v>1.56</v>
+        <v>0.95</v>
       </c>
       <c r="H34">
         <v>1.99</v>
@@ -11988,7 +12025,7 @@
         <v>0.73</v>
       </c>
       <c r="G35">
-        <v>3.08</v>
+        <v>0.94</v>
       </c>
       <c r="H35">
         <v>1.92</v>
@@ -12023,7 +12060,7 @@
         <v>0.73</v>
       </c>
       <c r="G36">
-        <v>1.9</v>
+        <v>0.98</v>
       </c>
       <c r="H36">
         <v>1.89</v>
@@ -12058,7 +12095,7 @@
         <v>0.82</v>
       </c>
       <c r="G37">
-        <v>2.08</v>
+        <v>0.98</v>
       </c>
       <c r="H37">
         <v>1.73</v>
@@ -12093,7 +12130,7 @@
         <v>1.35</v>
       </c>
       <c r="G38">
-        <v>1.94</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <v>2.37</v>
@@ -12128,7 +12165,7 @@
         <v>0.81</v>
       </c>
       <c r="G39">
-        <v>2</v>
+        <v>1.08</v>
       </c>
       <c r="H39">
         <v>1.75</v>
@@ -12163,7 +12200,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G40">
-        <v>2.11</v>
+        <v>0.9</v>
       </c>
       <c r="H40">
         <v>1.73</v>
@@ -12198,7 +12235,7 @@
         <v>1.08</v>
       </c>
       <c r="G41">
-        <v>1.53</v>
+        <v>0.98</v>
       </c>
       <c r="H41">
         <v>2.95</v>
@@ -12233,7 +12270,7 @@
         <v>0.98</v>
       </c>
       <c r="G42">
-        <v>1.83</v>
+        <v>1.5</v>
       </c>
       <c r="H42">
         <v>1.72</v>
@@ -12268,7 +12305,7 @@
         <v>0.83</v>
       </c>
       <c r="G43">
-        <v>1.87</v>
+        <v>1.54</v>
       </c>
       <c r="H43">
         <v>2.85</v>
@@ -12303,7 +12340,7 @@
         <v>0.82</v>
       </c>
       <c r="G44">
-        <v>3</v>
+        <v>1.69</v>
       </c>
       <c r="H44">
         <v>1.79</v>
@@ -12338,7 +12375,7 @@
         <v>0.89</v>
       </c>
       <c r="G45">
-        <v>2.31</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H45">
         <v>1.69</v>
@@ -12373,7 +12410,7 @@
         <v>0.86</v>
       </c>
       <c r="G46">
-        <v>1.75</v>
+        <v>1.28</v>
       </c>
       <c r="H46">
         <v>1.92</v>
@@ -12408,7 +12445,7 @@
         <v>0.78</v>
       </c>
       <c r="G47">
-        <v>1.84</v>
+        <v>0.92</v>
       </c>
       <c r="H47">
         <v>3.78</v>
@@ -12443,7 +12480,7 @@
         <v>0.69</v>
       </c>
       <c r="G48">
-        <v>2.4900000000000002</v>
+        <v>0.93</v>
       </c>
       <c r="H48">
         <v>1.93</v>
@@ -12478,7 +12515,7 @@
         <v>0.72</v>
       </c>
       <c r="G49">
-        <v>1.88</v>
+        <v>0.97</v>
       </c>
       <c r="H49">
         <v>2.72</v>
@@ -12513,7 +12550,7 @@
         <v>1.02</v>
       </c>
       <c r="G50">
-        <v>1.72</v>
+        <v>1.32</v>
       </c>
       <c r="H50">
         <v>2.4700000000000002</v>
@@ -12548,7 +12585,7 @@
         <v>1.04</v>
       </c>
       <c r="G51">
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="H51">
         <v>1.69</v>
@@ -12583,7 +12620,7 @@
         <v>0.74</v>
       </c>
       <c r="G52">
-        <v>1.74</v>
+        <v>0.94</v>
       </c>
       <c r="H52">
         <v>1.68</v>
@@ -12618,7 +12655,7 @@
         <v>0.87</v>
       </c>
       <c r="G53">
-        <v>2.37</v>
+        <v>1.05</v>
       </c>
       <c r="H53">
         <v>2.37</v>
@@ -12653,7 +12690,7 @@
         <v>0.82</v>
       </c>
       <c r="G54">
-        <v>1.78</v>
+        <v>0.94</v>
       </c>
       <c r="H54">
         <v>1.83</v>
@@ -12688,7 +12725,7 @@
         <v>0.81</v>
       </c>
       <c r="G55">
-        <v>1.59</v>
+        <v>1.22</v>
       </c>
       <c r="H55">
         <v>2.83</v>
@@ -12723,7 +12760,7 @@
         <v>0.8</v>
       </c>
       <c r="G56">
-        <v>2.6</v>
+        <v>0.95</v>
       </c>
       <c r="H56">
         <v>2.15</v>
@@ -12758,7 +12795,7 @@
         <v>0.93</v>
       </c>
       <c r="G57">
-        <v>2.61</v>
+        <v>1.04</v>
       </c>
       <c r="H57">
         <v>2.2400000000000002</v>
@@ -12793,7 +12830,7 @@
         <v>0.78</v>
       </c>
       <c r="G58">
-        <v>1.76</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="H58">
         <v>2.56</v>
@@ -12828,7 +12865,7 @@
         <v>1.78</v>
       </c>
       <c r="G59">
-        <v>2.23</v>
+        <v>1.41</v>
       </c>
       <c r="H59">
         <v>1.87</v>
@@ -12863,7 +12900,7 @@
         <v>1.2</v>
       </c>
       <c r="G60">
-        <v>2.31</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="H60">
         <v>1.86</v>
@@ -12898,7 +12935,7 @@
         <v>0.89</v>
       </c>
       <c r="G61">
-        <v>2.09</v>
+        <v>0.89</v>
       </c>
       <c r="H61">
         <v>2.23</v>
@@ -12933,7 +12970,7 @@
         <v>0.76</v>
       </c>
       <c r="G62">
-        <v>1.83</v>
+        <v>1.04</v>
       </c>
       <c r="H62">
         <v>2.4</v>
@@ -12968,7 +13005,7 @@
         <v>0.83</v>
       </c>
       <c r="G63">
-        <v>2.4700000000000002</v>
+        <v>1.08</v>
       </c>
       <c r="H63">
         <v>1.96</v>
@@ -13003,7 +13040,7 @@
         <v>0.87</v>
       </c>
       <c r="G64">
-        <v>2.88</v>
+        <v>1.17</v>
       </c>
       <c r="H64">
         <v>1.81</v>
@@ -13038,7 +13075,7 @@
         <v>0.85</v>
       </c>
       <c r="G65">
-        <v>1.73</v>
+        <v>1.25</v>
       </c>
       <c r="H65">
         <v>2.12</v>
@@ -13073,7 +13110,7 @@
         <v>0.81</v>
       </c>
       <c r="G66">
-        <v>2.5299999999999998</v>
+        <v>0.92</v>
       </c>
       <c r="H66">
         <v>1.75</v>
@@ -13108,7 +13145,7 @@
         <v>1.31</v>
       </c>
       <c r="G67">
-        <v>1.73</v>
+        <v>0.92</v>
       </c>
       <c r="H67">
         <v>1.59</v>
@@ -13143,7 +13180,7 @@
         <v>1.17</v>
       </c>
       <c r="G68">
-        <v>1.71</v>
+        <v>1.2</v>
       </c>
       <c r="H68">
         <v>1.6</v>
@@ -13178,7 +13215,7 @@
         <v>0.68</v>
       </c>
       <c r="G69">
-        <v>2.2599999999999998</v>
+        <v>1.26</v>
       </c>
       <c r="H69">
         <v>2.09</v>
@@ -13213,7 +13250,7 @@
         <v>0.82</v>
       </c>
       <c r="G70">
-        <v>2.19</v>
+        <v>1.03</v>
       </c>
       <c r="H70">
         <v>2.0099999999999998</v>
@@ -13248,7 +13285,7 @@
         <v>0.84</v>
       </c>
       <c r="G71">
-        <v>1.65</v>
+        <v>1.03</v>
       </c>
       <c r="H71">
         <v>1.56</v>
@@ -13283,7 +13320,7 @@
         <v>1.25</v>
       </c>
       <c r="G72">
-        <v>1.82</v>
+        <v>0.99</v>
       </c>
       <c r="H72">
         <v>1.66</v>
@@ -13318,7 +13355,7 @@
         <v>1.05</v>
       </c>
       <c r="G73">
-        <v>1.93</v>
+        <v>0.93</v>
       </c>
       <c r="H73">
         <v>1.76</v>
@@ -13353,7 +13390,7 @@
         <v>0.85</v>
       </c>
       <c r="G74">
-        <v>1.79</v>
+        <v>0.9</v>
       </c>
       <c r="H74">
         <v>2.42</v>
@@ -13388,7 +13425,7 @@
         <v>0.8</v>
       </c>
       <c r="G75">
-        <v>1.69</v>
+        <v>1.06</v>
       </c>
       <c r="H75">
         <v>1.57</v>
@@ -13423,7 +13460,7 @@
         <v>1.19</v>
       </c>
       <c r="G76">
-        <v>2.69</v>
+        <v>1.32</v>
       </c>
       <c r="H76">
         <v>1.92</v>
@@ -13458,7 +13495,7 @@
         <v>1.06</v>
       </c>
       <c r="G77">
-        <v>2.2799999999999998</v>
+        <v>0.94</v>
       </c>
       <c r="H77">
         <v>2.1</v>
@@ -13493,7 +13530,7 @@
         <v>0.74</v>
       </c>
       <c r="G78">
-        <v>1.66</v>
+        <v>1.06</v>
       </c>
       <c r="H78">
         <v>2.9</v>
@@ -13528,7 +13565,7 @@
         <v>0.82</v>
       </c>
       <c r="G79">
-        <v>2.2799999999999998</v>
+        <v>1.92</v>
       </c>
       <c r="H79">
         <v>3.46</v>
@@ -13563,7 +13600,7 @@
         <v>0.78</v>
       </c>
       <c r="G80">
-        <v>1.86</v>
+        <v>1.21</v>
       </c>
       <c r="H80">
         <v>1.68</v>
@@ -13598,7 +13635,7 @@
         <v>0.77</v>
       </c>
       <c r="G81">
-        <v>2.59</v>
+        <v>1.07</v>
       </c>
       <c r="H81">
         <v>1.95</v>
@@ -13633,7 +13670,7 @@
         <v>1.2</v>
       </c>
       <c r="G82">
-        <v>2.12</v>
+        <v>1.4</v>
       </c>
       <c r="H82">
         <v>2.93</v>
@@ -13668,7 +13705,7 @@
         <v>0.69</v>
       </c>
       <c r="G83">
-        <v>1.64</v>
+        <v>1.8</v>
       </c>
       <c r="H83">
         <v>1.98</v>
@@ -13703,7 +13740,7 @@
         <v>0.79</v>
       </c>
       <c r="G84">
-        <v>2.91</v>
+        <v>1.24</v>
       </c>
       <c r="H84">
         <v>2.41</v>
@@ -13738,7 +13775,7 @@
         <v>0.81</v>
       </c>
       <c r="G85">
-        <v>2.27</v>
+        <v>1.56</v>
       </c>
       <c r="H85">
         <v>1.67</v>
@@ -13773,7 +13810,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="G86">
-        <v>2.1800000000000002</v>
+        <v>1.03</v>
       </c>
       <c r="H86">
         <v>2.0099999999999998</v>
@@ -13808,7 +13845,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="G87">
-        <v>1.8</v>
+        <v>1.92</v>
       </c>
       <c r="H87">
         <v>1.77</v>
@@ -13843,7 +13880,7 @@
         <v>0.84</v>
       </c>
       <c r="G88">
-        <v>1.78</v>
+        <v>1.46</v>
       </c>
       <c r="H88">
         <v>2.67</v>
@@ -13878,7 +13915,7 @@
         <v>0.81</v>
       </c>
       <c r="G89">
-        <v>1.8</v>
+        <v>0.94</v>
       </c>
       <c r="H89">
         <v>1.96</v>
@@ -13913,7 +13950,7 @@
         <v>0.81</v>
       </c>
       <c r="G90">
-        <v>2.4700000000000002</v>
+        <v>0.93</v>
       </c>
       <c r="H90">
         <v>1.96</v>
@@ -13948,7 +13985,7 @@
         <v>0.82</v>
       </c>
       <c r="G91">
-        <v>2.2400000000000002</v>
+        <v>0.97</v>
       </c>
       <c r="H91">
         <v>1.87</v>
@@ -13983,7 +14020,7 @@
         <v>0.74</v>
       </c>
       <c r="G92">
-        <v>1.72</v>
+        <v>0.96</v>
       </c>
       <c r="H92">
         <v>1.55</v>
@@ -14018,7 +14055,7 @@
         <v>0.72</v>
       </c>
       <c r="G93">
-        <v>1.74</v>
+        <v>1.23</v>
       </c>
       <c r="H93">
         <v>2.39</v>
@@ -14053,7 +14090,7 @@
         <v>0.85</v>
       </c>
       <c r="G94">
-        <v>1.84</v>
+        <v>1.06</v>
       </c>
       <c r="H94">
         <v>2.62</v>
@@ -14088,7 +14125,7 @@
         <v>1.04</v>
       </c>
       <c r="G95">
-        <v>1.92</v>
+        <v>1.06</v>
       </c>
       <c r="H95">
         <v>2.5</v>
@@ -14123,7 +14160,7 @@
         <v>0.78</v>
       </c>
       <c r="G96">
-        <v>2.92</v>
+        <v>0.94</v>
       </c>
       <c r="H96">
         <v>2.4500000000000002</v>
@@ -14158,7 +14195,7 @@
         <v>1.05</v>
       </c>
       <c r="G97">
-        <v>1.65</v>
+        <v>0.92</v>
       </c>
       <c r="H97">
         <v>2.54</v>
@@ -14193,7 +14230,7 @@
         <v>0.9</v>
       </c>
       <c r="G98">
-        <v>1.78</v>
+        <v>0.95</v>
       </c>
       <c r="H98">
         <v>2.19</v>
@@ -14228,7 +14265,7 @@
         <v>0.75</v>
       </c>
       <c r="G99">
-        <v>2</v>
+        <v>1.29</v>
       </c>
       <c r="H99">
         <v>1.56</v>
@@ -14263,7 +14300,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="G100">
-        <v>1.98</v>
+        <v>1.07</v>
       </c>
       <c r="H100">
         <v>1.87</v>
@@ -14298,7 +14335,7 @@
         <v>0.98</v>
       </c>
       <c r="G101">
-        <v>1.75</v>
+        <v>0.92</v>
       </c>
       <c r="H101">
         <v>2.5099999999999998</v>
@@ -14342,7 +14379,7 @@
       </c>
       <c r="G103">
         <f t="shared" si="0"/>
-        <v>2.0390000000000001</v>
+        <v>1.1495000000000002</v>
       </c>
       <c r="H103">
         <f t="shared" si="0"/>
@@ -14391,7 +14428,7 @@
       </c>
       <c r="G104">
         <f t="shared" si="1"/>
-        <v>0.36672313614750257</v>
+        <v>0.3716394880672792</v>
       </c>
       <c r="H104">
         <f t="shared" si="1"/>
@@ -14440,7 +14477,7 @@
       </c>
       <c r="G106">
         <f t="shared" si="2"/>
-        <v>1.48</v>
+        <v>0.88</v>
       </c>
       <c r="H106">
         <f t="shared" si="2"/>
@@ -14489,7 +14526,7 @@
       </c>
       <c r="G107">
         <f t="shared" si="3"/>
-        <v>1.75</v>
+        <v>0.94</v>
       </c>
       <c r="H107">
         <f t="shared" si="3"/>
@@ -14538,7 +14575,7 @@
       </c>
       <c r="G108">
         <f t="shared" si="4"/>
-        <v>1.9350000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="H108">
         <f t="shared" si="4"/>
@@ -14587,7 +14624,7 @@
       </c>
       <c r="G109">
         <f t="shared" si="5"/>
-        <v>2.2624999999999997</v>
+        <v>1.2224999999999999</v>
       </c>
       <c r="H109">
         <f t="shared" si="5"/>
@@ -14636,7 +14673,7 @@
       </c>
       <c r="G110">
         <f t="shared" si="6"/>
-        <v>3.08</v>
+        <v>3.26</v>
       </c>
       <c r="H110">
         <f t="shared" si="6"/>
@@ -14685,7 +14722,7 @@
       </c>
       <c r="G112" s="3">
         <f t="shared" si="7"/>
-        <v>0.27</v>
+        <v>5.9999999999999942E-2</v>
       </c>
       <c r="H112" s="3">
         <f t="shared" si="7"/>
@@ -14737,7 +14774,7 @@
       </c>
       <c r="G113" s="1">
         <f t="shared" si="8"/>
-        <v>1.75</v>
+        <v>0.94</v>
       </c>
       <c r="H113" s="1">
         <f t="shared" si="8"/>
@@ -14789,7 +14826,7 @@
       </c>
       <c r="G114" s="1">
         <f t="shared" si="9"/>
-        <v>0.18500000000000005</v>
+        <v>9.000000000000008E-2</v>
       </c>
       <c r="H114" s="1">
         <f t="shared" si="9"/>
@@ -14841,7 +14878,7 @@
       </c>
       <c r="G115" s="1">
         <f t="shared" si="9"/>
-        <v>0.32749999999999968</v>
+        <v>0.19249999999999989</v>
       </c>
       <c r="H115" s="1">
         <f t="shared" si="9"/>
@@ -14893,7 +14930,7 @@
       </c>
       <c r="G116" s="2">
         <f t="shared" si="9"/>
-        <v>0.81750000000000034</v>
+        <v>2.0374999999999996</v>
       </c>
       <c r="H116" s="2">
         <f t="shared" si="9"/>
@@ -14936,8 +14973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M116"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -15001,7 +15038,7 @@
         <v>0.35</v>
       </c>
       <c r="G2">
-        <v>1.85</v>
+        <v>0.98</v>
       </c>
       <c r="H2">
         <v>2.14</v>
@@ -15036,7 +15073,7 @@
         <v>0.35</v>
       </c>
       <c r="G3">
-        <v>1.37</v>
+        <v>0.64</v>
       </c>
       <c r="H3">
         <v>2.37</v>
@@ -15071,7 +15108,7 @@
         <v>0.35</v>
       </c>
       <c r="G4">
-        <v>1.77</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H4">
         <v>1.43</v>
@@ -15106,7 +15143,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="G5">
-        <v>1.51</v>
+        <v>0.77</v>
       </c>
       <c r="H5">
         <v>2.0499999999999998</v>
@@ -15141,7 +15178,7 @@
         <v>0.45</v>
       </c>
       <c r="G6">
-        <v>2.0099999999999998</v>
+        <v>0.67</v>
       </c>
       <c r="H6">
         <v>1.57</v>
@@ -15176,7 +15213,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G7">
-        <v>2.13</v>
+        <v>1.46</v>
       </c>
       <c r="H7">
         <v>1.46</v>
@@ -15211,7 +15248,7 @@
         <v>0.31</v>
       </c>
       <c r="G8">
-        <v>2.02</v>
+        <v>0.59</v>
       </c>
       <c r="H8">
         <v>1.65</v>
@@ -15246,7 +15283,7 @@
         <v>0.32</v>
       </c>
       <c r="G9">
-        <v>1.65</v>
+        <v>0.68</v>
       </c>
       <c r="H9">
         <v>2.35</v>
@@ -15281,7 +15318,7 @@
         <v>0.54</v>
       </c>
       <c r="G10">
-        <v>1.75</v>
+        <v>1.99</v>
       </c>
       <c r="H10">
         <v>2.38</v>
@@ -15316,7 +15353,7 @@
         <v>0.31</v>
       </c>
       <c r="G11">
-        <v>2.31</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H11">
         <v>1.86</v>
@@ -15351,7 +15388,7 @@
         <v>0.37</v>
       </c>
       <c r="G12">
-        <v>1.51</v>
+        <v>0.61</v>
       </c>
       <c r="H12">
         <v>1.54</v>
@@ -15386,7 +15423,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="G13">
-        <v>1.44</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H13">
         <v>1.58</v>
@@ -15421,7 +15458,7 @@
         <v>0.43</v>
       </c>
       <c r="G14">
-        <v>1.4</v>
+        <v>0.71</v>
       </c>
       <c r="H14">
         <v>1.82</v>
@@ -15456,7 +15493,7 @@
         <v>0.32</v>
       </c>
       <c r="G15">
-        <v>1.86</v>
+        <v>0.68</v>
       </c>
       <c r="H15">
         <v>2.37</v>
@@ -15491,7 +15528,7 @@
         <v>0.42</v>
       </c>
       <c r="G16">
-        <v>1.82</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H16">
         <v>1.58</v>
@@ -15526,7 +15563,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G17">
-        <v>1.84</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H17">
         <v>1.98</v>
@@ -15561,7 +15598,7 @@
         <v>0.37</v>
       </c>
       <c r="G18">
-        <v>1.6</v>
+        <v>0.63</v>
       </c>
       <c r="H18">
         <v>1.48</v>
@@ -15596,7 +15633,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G19">
-        <v>4.3899999999999997</v>
+        <v>0.81</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -15631,7 +15668,7 @@
         <v>0.36</v>
       </c>
       <c r="G20">
-        <v>2.19</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H20">
         <v>1.43</v>
@@ -15666,7 +15703,7 @@
         <v>0.34</v>
       </c>
       <c r="G21">
-        <v>1.46</v>
+        <v>0.65</v>
       </c>
       <c r="H21">
         <v>1.34</v>
@@ -15701,7 +15738,7 @@
         <v>0.49</v>
       </c>
       <c r="G22">
-        <v>1.89</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H22">
         <v>1.27</v>
@@ -15736,7 +15773,7 @@
         <v>0.41</v>
       </c>
       <c r="G23">
-        <v>2.2799999999999998</v>
+        <v>0.74</v>
       </c>
       <c r="H23">
         <v>1.7</v>
@@ -15771,7 +15808,7 @@
         <v>0.45</v>
       </c>
       <c r="G24">
-        <v>1.7</v>
+        <v>0.61</v>
       </c>
       <c r="H24">
         <v>1.6</v>
@@ -15806,7 +15843,7 @@
         <v>0.45</v>
       </c>
       <c r="G25">
-        <v>1.44</v>
+        <v>0.59</v>
       </c>
       <c r="H25">
         <v>1.46</v>
@@ -15841,7 +15878,7 @@
         <v>0.31</v>
       </c>
       <c r="G26">
-        <v>1.57</v>
+        <v>0.6</v>
       </c>
       <c r="H26">
         <v>1.81</v>
@@ -15876,7 +15913,7 @@
         <v>0.4</v>
       </c>
       <c r="G27">
-        <v>1.63</v>
+        <v>0.6</v>
       </c>
       <c r="H27">
         <v>1.69</v>
@@ -15911,7 +15948,7 @@
         <v>0.34</v>
       </c>
       <c r="G28">
-        <v>2.23</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H28">
         <v>2.0699999999999998</v>
@@ -15946,7 +15983,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="G29">
-        <v>1.55</v>
+        <v>0.71</v>
       </c>
       <c r="H29">
         <v>1.96</v>
@@ -15981,7 +16018,7 @@
         <v>0.49</v>
       </c>
       <c r="G30">
-        <v>1.49</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H30">
         <v>1.93</v>
@@ -16016,7 +16053,7 @@
         <v>0.31</v>
       </c>
       <c r="G31">
-        <v>2.06</v>
+        <v>0.68</v>
       </c>
       <c r="H31">
         <v>1.9</v>
@@ -16051,7 +16088,7 @@
         <v>0.38</v>
       </c>
       <c r="G32">
-        <v>1.41</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H32">
         <v>2.0699999999999998</v>
@@ -16086,7 +16123,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G33">
-        <v>1.55</v>
+        <v>0.82</v>
       </c>
       <c r="H33">
         <v>1.59</v>
@@ -16121,7 +16158,7 @@
         <v>0.46</v>
       </c>
       <c r="G34">
-        <v>1.54</v>
+        <v>0.72</v>
       </c>
       <c r="H34">
         <v>1.7</v>
@@ -16156,7 +16193,7 @@
         <v>0.34</v>
       </c>
       <c r="G35">
-        <v>1.58</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="H35">
         <v>1.47</v>
@@ -16191,7 +16228,7 @@
         <v>0.35</v>
       </c>
       <c r="G36">
-        <v>1.56</v>
+        <v>0.71</v>
       </c>
       <c r="H36">
         <v>1.89</v>
@@ -16226,7 +16263,7 @@
         <v>0.35</v>
       </c>
       <c r="G37">
-        <v>1.46</v>
+        <v>0.65</v>
       </c>
       <c r="H37">
         <v>1.99</v>
@@ -16261,7 +16298,7 @@
         <v>0.37</v>
       </c>
       <c r="G38">
-        <v>1.72</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H38">
         <v>1.96</v>
@@ -16296,7 +16333,7 @@
         <v>0.44</v>
       </c>
       <c r="G39">
-        <v>1.23</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H39">
         <v>1.92</v>
@@ -16331,7 +16368,7 @@
         <v>0.49</v>
       </c>
       <c r="G40">
-        <v>2.2200000000000002</v>
+        <v>1.61</v>
       </c>
       <c r="H40">
         <v>1.36</v>
@@ -16366,7 +16403,7 @@
         <v>0.34</v>
       </c>
       <c r="G41">
-        <v>1.59</v>
+        <v>0.64</v>
       </c>
       <c r="H41">
         <v>2.4</v>
@@ -16401,7 +16438,7 @@
         <v>0.3</v>
       </c>
       <c r="G42">
-        <v>1.62</v>
+        <v>0.6</v>
       </c>
       <c r="H42">
         <v>2.1</v>
@@ -16436,7 +16473,7 @@
         <v>0.36</v>
       </c>
       <c r="G43">
-        <v>1.9</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H43">
         <v>2.21</v>
@@ -16471,7 +16508,7 @@
         <v>0.37</v>
       </c>
       <c r="G44">
-        <v>1.69</v>
+        <v>0.62</v>
       </c>
       <c r="H44">
         <v>1.1499999999999999</v>
@@ -16506,7 +16543,7 @@
         <v>0.45</v>
       </c>
       <c r="G45">
-        <v>1.53</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H45">
         <v>1.99</v>
@@ -16541,7 +16578,7 @@
         <v>0.35</v>
       </c>
       <c r="G46">
-        <v>1.6</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H46">
         <v>1.98</v>
@@ -16576,7 +16613,7 @@
         <v>0.37</v>
       </c>
       <c r="G47">
-        <v>1.59</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H47">
         <v>2.34</v>
@@ -16611,7 +16648,7 @@
         <v>0.34</v>
       </c>
       <c r="G48">
-        <v>2.72</v>
+        <v>0.71</v>
       </c>
       <c r="H48">
         <v>1.62</v>
@@ -16646,7 +16683,7 @@
         <v>0.45</v>
       </c>
       <c r="G49">
-        <v>1.46</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H49">
         <v>1.47</v>
@@ -16681,7 +16718,7 @@
         <v>0.35</v>
       </c>
       <c r="G50">
-        <v>1.42</v>
+        <v>0.89</v>
       </c>
       <c r="H50">
         <v>1.45</v>
@@ -16716,7 +16753,7 @@
         <v>0.32</v>
       </c>
       <c r="G51">
-        <v>2.14</v>
+        <v>0.62</v>
       </c>
       <c r="H51">
         <v>1.34</v>
@@ -16751,7 +16788,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G52">
-        <v>1.41</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H52">
         <v>1.42</v>
@@ -16786,7 +16823,7 @@
         <v>0.36</v>
       </c>
       <c r="G53">
-        <v>2.02</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H53">
         <v>1.58</v>
@@ -16821,7 +16858,7 @@
         <v>0.36</v>
       </c>
       <c r="G54">
-        <v>1.53</v>
+        <v>1</v>
       </c>
       <c r="H54">
         <v>2.11</v>
@@ -16856,7 +16893,7 @@
         <v>0.36</v>
       </c>
       <c r="G55">
-        <v>2.13</v>
+        <v>0.74</v>
       </c>
       <c r="H55">
         <v>2</v>
@@ -16891,7 +16928,7 @@
         <v>0.54</v>
       </c>
       <c r="G56">
-        <v>2.27</v>
+        <v>0.61</v>
       </c>
       <c r="H56">
         <v>1.6</v>
@@ -16926,7 +16963,7 @@
         <v>0.34</v>
       </c>
       <c r="G57">
-        <v>1.86</v>
+        <v>0.61</v>
       </c>
       <c r="H57">
         <v>2.4300000000000002</v>
@@ -16961,7 +16998,7 @@
         <v>0.3</v>
       </c>
       <c r="G58">
-        <v>1.96</v>
+        <v>0.86</v>
       </c>
       <c r="H58">
         <v>2.16</v>
@@ -16996,7 +17033,7 @@
         <v>0.32</v>
       </c>
       <c r="G59">
-        <v>2.08</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="H59">
         <v>1.36</v>
@@ -17031,7 +17068,7 @@
         <v>0.34</v>
       </c>
       <c r="G60">
-        <v>2.7</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H60">
         <v>2.29</v>
@@ -17066,7 +17103,7 @@
         <v>0.3</v>
       </c>
       <c r="G61">
-        <v>3.06</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H61">
         <v>1.7</v>
@@ -17101,7 +17138,7 @@
         <v>0.3</v>
       </c>
       <c r="G62">
-        <v>1.7</v>
+        <v>0.66</v>
       </c>
       <c r="H62">
         <v>1.51</v>
@@ -17136,7 +17173,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G63">
-        <v>1.47</v>
+        <v>0.61</v>
       </c>
       <c r="H63">
         <v>1.98</v>
@@ -17171,7 +17208,7 @@
         <v>0.35</v>
       </c>
       <c r="G64">
-        <v>2.16</v>
+        <v>0.65</v>
       </c>
       <c r="H64">
         <v>2.11</v>
@@ -17206,7 +17243,7 @@
         <v>0.44</v>
       </c>
       <c r="G65">
-        <v>1.6</v>
+        <v>0.65</v>
       </c>
       <c r="H65">
         <v>2.06</v>
@@ -17241,7 +17278,7 @@
         <v>0.33</v>
       </c>
       <c r="G66">
-        <v>1.48</v>
+        <v>0.74</v>
       </c>
       <c r="H66">
         <v>1.64</v>
@@ -17276,7 +17313,7 @@
         <v>0.32</v>
       </c>
       <c r="G67">
-        <v>2.1800000000000002</v>
+        <v>0.72</v>
       </c>
       <c r="H67">
         <v>1.99</v>
@@ -17311,7 +17348,7 @@
         <v>0.53</v>
       </c>
       <c r="G68">
-        <v>2.15</v>
+        <v>0.61</v>
       </c>
       <c r="H68">
         <v>1.55</v>
@@ -17346,7 +17383,7 @@
         <v>0.34</v>
       </c>
       <c r="G69">
-        <v>1.45</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H69">
         <v>1.77</v>
@@ -17381,7 +17418,7 @@
         <v>0.34</v>
       </c>
       <c r="G70">
-        <v>1.58</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H70">
         <v>1.64</v>
@@ -17416,7 +17453,7 @@
         <v>0.51</v>
       </c>
       <c r="G71">
-        <v>1.6</v>
+        <v>0.65</v>
       </c>
       <c r="H71">
         <v>3.58</v>
@@ -17451,7 +17488,7 @@
         <v>0.53</v>
       </c>
       <c r="G72">
-        <v>1.46</v>
+        <v>0.61</v>
       </c>
       <c r="H72">
         <v>1.37</v>
@@ -17486,7 +17523,7 @@
         <v>0.31</v>
       </c>
       <c r="G73">
-        <v>1.72</v>
+        <v>0.69</v>
       </c>
       <c r="H73">
         <v>1.94</v>
@@ -17521,7 +17558,7 @@
         <v>0.36</v>
       </c>
       <c r="G74">
-        <v>2.1</v>
+        <v>0.62</v>
       </c>
       <c r="H74">
         <v>1.76</v>
@@ -17556,7 +17593,7 @@
         <v>0.36</v>
       </c>
       <c r="G75">
-        <v>1.42</v>
+        <v>0.66</v>
       </c>
       <c r="H75">
         <v>1.76</v>
@@ -17591,7 +17628,7 @@
         <v>0.33</v>
       </c>
       <c r="G76">
-        <v>2.0299999999999998</v>
+        <v>0.97</v>
       </c>
       <c r="H76">
         <v>1.87</v>
@@ -17626,7 +17663,7 @@
         <v>0.35</v>
       </c>
       <c r="G77">
-        <v>1.67</v>
+        <v>0.72</v>
       </c>
       <c r="H77">
         <v>1.45</v>
@@ -17661,7 +17698,7 @@
         <v>0.41</v>
       </c>
       <c r="G78">
-        <v>1.56</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H78">
         <v>1.92</v>
@@ -17696,7 +17733,7 @@
         <v>0.37</v>
       </c>
       <c r="G79">
-        <v>1.61</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H79">
         <v>1.55</v>
@@ -17731,7 +17768,7 @@
         <v>0.48</v>
       </c>
       <c r="G80">
-        <v>1.64</v>
+        <v>0.6</v>
       </c>
       <c r="H80">
         <v>1.95</v>
@@ -17766,7 +17803,7 @@
         <v>0.33</v>
       </c>
       <c r="G81">
-        <v>1.64</v>
+        <v>0.69</v>
       </c>
       <c r="H81">
         <v>1.47</v>
@@ -17801,7 +17838,7 @@
         <v>0.49</v>
       </c>
       <c r="G82">
-        <v>1.87</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H82">
         <v>1.52</v>
@@ -17836,7 +17873,7 @@
         <v>0.38</v>
       </c>
       <c r="G83">
-        <v>1.42</v>
+        <v>0.8</v>
       </c>
       <c r="H83">
         <v>1.96</v>
@@ -17871,7 +17908,7 @@
         <v>0.36</v>
       </c>
       <c r="G84">
-        <v>1.24</v>
+        <v>0.65</v>
       </c>
       <c r="H84">
         <v>2.31</v>
@@ -17906,7 +17943,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G85">
-        <v>2.02</v>
+        <v>0.62</v>
       </c>
       <c r="H85">
         <v>2.19</v>
@@ -17941,7 +17978,7 @@
         <v>0.36</v>
       </c>
       <c r="G86">
-        <v>1.57</v>
+        <v>0.61</v>
       </c>
       <c r="H86">
         <v>1.63</v>
@@ -17976,7 +18013,7 @@
         <v>0.36</v>
       </c>
       <c r="G87">
-        <v>1.44</v>
+        <v>0.96</v>
       </c>
       <c r="H87">
         <v>2.0699999999999998</v>
@@ -18011,7 +18048,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="G88">
-        <v>1.48</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H88">
         <v>2</v>
@@ -18046,7 +18083,7 @@
         <v>0.48</v>
       </c>
       <c r="G89">
-        <v>1.42</v>
+        <v>0.59</v>
       </c>
       <c r="H89">
         <v>1.36</v>
@@ -18081,7 +18118,7 @@
         <v>0.45</v>
       </c>
       <c r="G90">
-        <v>2.09</v>
+        <v>0.59</v>
       </c>
       <c r="H90">
         <v>1.64</v>
@@ -18116,7 +18153,7 @@
         <v>0.37</v>
       </c>
       <c r="G91">
-        <v>1.44</v>
+        <v>0.69</v>
       </c>
       <c r="H91">
         <v>1.94</v>
@@ -18151,7 +18188,7 @@
         <v>0.36</v>
       </c>
       <c r="G92">
-        <v>1.51</v>
+        <v>0.61</v>
       </c>
       <c r="H92">
         <v>1.44</v>
@@ -18186,7 +18223,7 @@
         <v>0.34</v>
       </c>
       <c r="G93">
-        <v>2.09</v>
+        <v>0.96</v>
       </c>
       <c r="H93">
         <v>1.81</v>
@@ -18221,7 +18258,7 @@
         <v>0.49</v>
       </c>
       <c r="G94">
-        <v>1.93</v>
+        <v>0.92</v>
       </c>
       <c r="H94">
         <v>5.54</v>
@@ -18256,7 +18293,7 @@
         <v>0.45</v>
       </c>
       <c r="G95">
-        <v>1.67</v>
+        <v>0.62</v>
       </c>
       <c r="H95">
         <v>1.52</v>
@@ -18291,7 +18328,7 @@
         <v>0.33</v>
       </c>
       <c r="G96">
-        <v>1.46</v>
+        <v>0.81</v>
       </c>
       <c r="H96">
         <v>1.85</v>
@@ -18326,7 +18363,7 @@
         <v>0.46</v>
       </c>
       <c r="G97">
-        <v>1.54</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H97">
         <v>1.3</v>
@@ -18361,7 +18398,7 @@
         <v>0.35</v>
       </c>
       <c r="G98">
-        <v>1.31</v>
+        <v>0.84</v>
       </c>
       <c r="H98">
         <v>3.96</v>
@@ -18396,7 +18433,7 @@
         <v>0.38</v>
       </c>
       <c r="G99">
-        <v>1.61</v>
+        <v>1.06</v>
       </c>
       <c r="H99">
         <v>1.72</v>
@@ -18431,7 +18468,7 @@
         <v>0.35</v>
       </c>
       <c r="G100">
-        <v>1.71</v>
+        <v>1.19</v>
       </c>
       <c r="H100">
         <v>1.39</v>
@@ -18466,7 +18503,7 @@
         <v>0.33</v>
       </c>
       <c r="G101">
-        <v>2</v>
+        <v>0.6</v>
       </c>
       <c r="H101">
         <v>1.4</v>
@@ -18510,7 +18547,7 @@
       </c>
       <c r="G103">
         <f t="shared" si="0"/>
-        <v>1.7730999999999995</v>
+        <v>0.72499999999999976</v>
       </c>
       <c r="H103">
         <f t="shared" si="0"/>
@@ -18559,7 +18596,7 @@
       </c>
       <c r="G104">
         <f t="shared" si="1"/>
-        <v>0.42466551305680622</v>
+        <v>0.27058298452628582</v>
       </c>
       <c r="H104">
         <f t="shared" si="1"/>
@@ -18608,7 +18645,7 @@
       </c>
       <c r="G106">
         <f t="shared" si="2"/>
-        <v>1.23</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H106">
         <f t="shared" si="2"/>
@@ -18657,7 +18694,7 @@
       </c>
       <c r="G107">
         <f t="shared" si="3"/>
-        <v>1.5049999999999999</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H107">
         <f t="shared" si="3"/>
@@ -18706,7 +18743,7 @@
       </c>
       <c r="G108">
         <f t="shared" si="4"/>
-        <v>1.6349999999999998</v>
+        <v>0.625</v>
       </c>
       <c r="H108">
         <f t="shared" si="4"/>
@@ -18755,7 +18792,7 @@
       </c>
       <c r="G109">
         <f t="shared" si="5"/>
-        <v>2.0124999999999997</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="H109">
         <f t="shared" si="5"/>
@@ -18804,7 +18841,7 @@
       </c>
       <c r="G110">
         <f t="shared" si="6"/>
-        <v>4.3899999999999997</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H110">
         <f t="shared" si="6"/>
@@ -18853,7 +18890,7 @@
       </c>
       <c r="G112" s="3">
         <f t="shared" si="7"/>
-        <v>0.27499999999999991</v>
+        <v>2.9999999999999916E-2</v>
       </c>
       <c r="H112" s="3">
         <f t="shared" si="7"/>
@@ -18905,7 +18942,7 @@
       </c>
       <c r="G113" s="1">
         <f t="shared" si="8"/>
-        <v>1.5049999999999999</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H113" s="1">
         <f t="shared" si="8"/>
@@ -18957,7 +18994,7 @@
       </c>
       <c r="G114" s="1">
         <f t="shared" si="9"/>
-        <v>0.12999999999999989</v>
+        <v>4.500000000000004E-2</v>
       </c>
       <c r="H114" s="1">
         <f t="shared" si="9"/>
@@ -19009,7 +19046,7 @@
       </c>
       <c r="G115" s="1">
         <f t="shared" si="9"/>
-        <v>0.37749999999999995</v>
+        <v>9.9999999999999978E-2</v>
       </c>
       <c r="H115" s="1">
         <f t="shared" si="9"/>
@@ -19061,7 +19098,7 @@
       </c>
       <c r="G116" s="2">
         <f t="shared" si="9"/>
-        <v>2.3774999999999999</v>
+        <v>1.4750000000000001</v>
       </c>
       <c r="H116" s="2">
         <f t="shared" si="9"/>
@@ -19104,7 +19141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
@@ -19126,8 +19163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="N127" sqref="N127"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103:A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20765,7 +20802,7 @@
         <v>18.383499999999998</v>
       </c>
       <c r="F103">
-        <f t="shared" ref="D103:G103" si="4">AVERAGE(F2:F101)</f>
+        <f t="shared" ref="F103:G103" si="4">AVERAGE(F2:F101)</f>
         <v>0.67342792956768394</v>
       </c>
       <c r="G103">
@@ -20786,7 +20823,7 @@
         <v>3.7660831875780074</v>
       </c>
       <c r="F104">
-        <f t="shared" ref="D104:G104" si="5">STDEV(F2:F101)</f>
+        <f t="shared" ref="F104:G104" si="5">STDEV(F2:F101)</f>
         <v>0.130699229921663</v>
       </c>
       <c r="G104">
@@ -20807,7 +20844,7 @@
         <v>14.53</v>
       </c>
       <c r="F106">
-        <f t="shared" ref="D106:G106" si="6">MIN(F2:F101)</f>
+        <f t="shared" ref="F106:G106" si="6">MIN(F2:F101)</f>
         <v>0.36823935558112769</v>
       </c>
       <c r="G106">
@@ -20828,7 +20865,7 @@
         <v>15.9175</v>
       </c>
       <c r="F107">
-        <f t="shared" ref="D107:G107" si="7">_xlfn.QUARTILE.INC(F2:F101,1)</f>
+        <f t="shared" ref="F107:G107" si="7">_xlfn.QUARTILE.INC(F2:F101,1)</f>
         <v>0.5842187182424935</v>
       </c>
       <c r="G107">
@@ -20849,7 +20886,7 @@
         <v>17.510000000000002</v>
       </c>
       <c r="F108">
-        <f t="shared" ref="D108:G108" si="8">MEDIAN(F2:F101)</f>
+        <f t="shared" ref="F108:G108" si="8">MEDIAN(F2:F101)</f>
         <v>0.69016070757472581</v>
       </c>
       <c r="G108">
@@ -20870,7 +20907,7 @@
         <v>19.295000000000002</v>
       </c>
       <c r="F109">
-        <f t="shared" ref="D109:G109" si="9">_xlfn.QUARTILE.INC(F2:F101,3)</f>
+        <f t="shared" ref="F109:G109" si="9">_xlfn.QUARTILE.INC(F2:F101,3)</f>
         <v>0.77165310184363234</v>
       </c>
       <c r="G109">
@@ -20891,7 +20928,7 @@
         <v>36.44</v>
       </c>
       <c r="F110">
-        <f t="shared" ref="D110:G110" si="10">MAX(F2:F101)</f>
+        <f t="shared" ref="F110:G110" si="10">MAX(F2:F101)</f>
         <v>0.92539039907460963</v>
       </c>
       <c r="G110">

</xml_diff>